<commit_message>
EBEGU-408: Statistiken Kanton implementieren inklusive Sichtbarkeit je Rolle
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -10,11 +10,19 @@
     <sheet name="Data" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="anteilMonat">Data!$L$9</definedName>
     <definedName name="bgPensum">Data!$G$9</definedName>
     <definedName name="elternbeitrag">Data!$O$9</definedName>
+    <definedName name="geburtsdatum">Data!$D$9</definedName>
+    <definedName name="monatsanfang">Data!$H$9</definedName>
+    <definedName name="monatsende">Data!$I$9</definedName>
+    <definedName name="nettotageIntervall">Data!$K$9</definedName>
+    <definedName name="nettotageMonat">Data!$J$9</definedName>
     <definedName name="platzbelegungAufgrundTage">Data!$M$9</definedName>
     <definedName name="verguenstigung">Data!$P$9</definedName>
     <definedName name="vollkosten">Data!$N$9</definedName>
+    <definedName name="zeitabschnittBis">Data!$F$9</definedName>
+    <definedName name="zeitabschnittVon">Data!$E$9</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -328,6 +336,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -351,12 +365,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -664,10 +672,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="H17" sqref="H16:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -680,9 +688,9 @@
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
     <col min="13" max="13" width="16" style="6" customWidth="1"/>
     <col min="14" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
@@ -740,64 +748,64 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="24" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="24"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="20" t="s">
+      <c r="O7" s="26"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="9" t="s">
         <v>18</v>
       </c>
@@ -807,7 +815,7 @@
       <c r="L8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="26"/>
+      <c r="M8" s="28"/>
       <c r="N8" s="18" t="s">
         <v>9</v>
       </c>
@@ -817,9 +825,9 @@
       <c r="P8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="5" t="s">
@@ -844,31 +852,31 @@
         <v>31</v>
       </c>
       <c r="H9" s="12" t="e">
-        <f t="shared" ref="H9" si="0">E9-DAY(E9)+1</f>
+        <f>zeitabschnittVon-DAY(zeitabschnittVon)+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="I9" s="12" t="e">
-        <f t="shared" ref="I9" si="1">EOMONTH(E9,0)</f>
+        <f>EOMONTH(zeitabschnittVon,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="J9" s="14" t="e">
-        <f t="shared" ref="J9" si="2">NETWORKDAYS(H9,I9)</f>
+        <f>NETWORKDAYS(monatsanfang,monatsende)</f>
         <v>#VALUE!</v>
       </c>
       <c r="K9" s="14" t="e">
-        <f t="shared" ref="K9" si="3">NETWORKDAYS(E9,F9)</f>
+        <f>NETWORKDAYS(zeitabschnittVon,zeitabschnittBis)</f>
         <v>#VALUE!</v>
       </c>
       <c r="L9" s="14" t="e">
-        <f t="shared" ref="L9" si="4">K9/J9</f>
+        <f>nettotageIntervall/nettotageMonat</f>
         <v>#VALUE!</v>
       </c>
       <c r="M9" s="13" t="e">
-        <f t="shared" ref="M9" si="5">G9*L9</f>
+        <f>bgPensum*anteilMonat</f>
         <v>#VALUE!</v>
       </c>
       <c r="N9" s="15" t="e">
-        <f>O9+P9</f>
+        <f>elternbeitrag+verguenstigung</f>
         <v>#VALUE!</v>
       </c>
       <c r="O9" s="16" t="s">
@@ -878,7 +886,7 @@
         <v>33</v>
       </c>
       <c r="Q9" t="e">
-        <f>IF(E9&gt;EOMONTH(D9,12),"Nein","Ja")</f>
+        <f>IF(zeitabschnittVon&gt;EOMONTH(geburtsdatum,12),"Nein","Ja")</f>
         <v>#VALUE!</v>
       </c>
       <c r="R9" s="5" t="s">
@@ -900,7 +908,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="27">
+      <c r="G10" s="19">
         <f>SUM(bgPensum)</f>
         <v>0</v>
       </c>
@@ -909,19 +917,19 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="27" t="e">
+      <c r="M10" s="19" t="e">
         <f>SUM(platzbelegungAufgrundTage)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N10" s="28" t="e">
+      <c r="N10" s="20" t="e">
         <f>SUM(vollkosten)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="20">
         <f>SUM(elternbeitrag)</f>
         <v>0</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="20">
         <f>SUM(verguenstigung)</f>
         <v>0</v>
       </c>
@@ -931,6 +939,10 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
EBEGU-408: Statistiken Kanton implementieren inklusive Sichtbarkeit je Rolle: Sortierung und teilweise Spalten ausblenden
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Kanton.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Kanton.xlsx
@@ -285,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,9 +323,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -358,6 +355,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,7 +671,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -681,9 +684,9 @@
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="16" style="6" customWidth="1"/>
     <col min="14" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
@@ -741,86 +744,86 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="28" t="s">
+      <c r="J7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="22" t="s">
+      <c r="O7" s="25"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="S7" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="28"/>
-      <c r="N8" s="18" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="5" t="s">
@@ -901,7 +904,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <f>SUM(bgPensum)</f>
         <v>0</v>
       </c>
@@ -910,19 +913,19 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="19" t="e">
+      <c r="M10" s="18" t="e">
         <f>SUM(platzbelegungAufgrundTage)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N10" s="20" t="e">
+      <c r="N10" s="19" t="e">
         <f>SUM(vollkosten)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="19">
         <f>SUM(elternbeitrag)</f>
         <v>0</v>
       </c>
-      <c r="P10" s="20">
+      <c r="P10" s="19">
         <f>SUM(verguenstigung)</f>
         <v>0</v>
       </c>
@@ -938,7 +941,8 @@
       <c r="L16" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="Q7:Q8"/>
@@ -953,6 +957,8 @@
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>